<commit_message>
Refer to ~Refunds web site on code engine
</commit_message>
<xml_diff>
--- a/artefacts/data/refunds.xlsx
+++ b/artefacts/data/refunds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\github\refundBot\artefacts\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RPA\github\refundBot\artefacts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2913E18-A7CE-4965-9353-0EBA635B7BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E037DAAE-9056-45CB-A714-B2E36647371E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="15360" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tickets" sheetId="3" r:id="rId1"/>
@@ -25,6 +25,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -284,162 +286,142 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -455,42 +437,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79995117038483843"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79995117038483843"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79995117038483843"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79995117038483843"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -502,123 +484,123 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.39994506668294322"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39994506668294322"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39994506668294322"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -628,6 +610,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -653,22 +665,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,45 +711,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -740,81 +722,79 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="7"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="29"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="34"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="37"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="29" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="29" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="29" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="37" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="18" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="29" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="29" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="37" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="37" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="37" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="20" fillId="4" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="21" fillId="2" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="37" applyFont="1"/>
+    <xf numFmtId="22" fontId="7" fillId="3" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="34" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -922,32 +902,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
       <c:rotY val="0"/>
-      <c:depthPercent val="100"/>
       <c:rAngAx val="0"/>
     </c:view3D>
     <c:floor>
@@ -958,7 +917,6 @@
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
-        <a:sp3d/>
       </c:spPr>
     </c:floor>
     <c:sideWall>
@@ -969,7 +927,6 @@
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
-        <a:sp3d/>
       </c:spPr>
     </c:sideWall>
     <c:backWall>
@@ -980,7 +937,6 @@
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
-        <a:sp3d/>
       </c:spPr>
     </c:backWall>
     <c:plotArea>
@@ -1011,7 +967,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-F69D-4EA7-B593-EC91C208A0F5}"/>
+                <c16:uniqueId val="{00000001-FBF5-4C8C-86F1-F322F184D29F}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1036,7 +992,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-F69D-4EA7-B593-EC91C208A0F5}"/>
+                <c16:uniqueId val="{00000003-FBF5-4C8C-86F1-F322F184D29F}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1061,7 +1017,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-F69D-4EA7-B593-EC91C208A0F5}"/>
+                <c16:uniqueId val="{00000005-FBF5-4C8C-86F1-F322F184D29F}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1086,7 +1042,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-F69D-4EA7-B593-EC91C208A0F5}"/>
+                <c16:uniqueId val="{00000007-FBF5-4C8C-86F1-F322F184D29F}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1111,7 +1067,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-F69D-4EA7-B593-EC91C208A0F5}"/>
+                <c16:uniqueId val="{00000009-FBF5-4C8C-86F1-F322F184D29F}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1136,7 +1092,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-F4D9-4334-96EB-A77F94DC2AB9}"/>
+                <c16:uniqueId val="{0000000B-FBF5-4C8C-86F1-F322F184D29F}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1195,7 +1151,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-051D-4033-BB44-BDBC13F63061}"/>
+              <c16:uniqueId val="{0000000C-FBF5-4C8C-86F1-F322F184D29F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1250,20 +1206,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln w="9525" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
@@ -1292,573 +1241,14 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>119062</xdr:colOff>
+      <xdr:colOff>118745</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
@@ -1871,7 +1261,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5387D8A-8950-4918-B2FC-0A069AB05761}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2069,6 +1459,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -2095,24 +1486,25 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2173,26 +1565,22 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05048FD4-FE6B-4DFE-B6DC-9425F4DD8CDF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:M2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2201,55 +1589,55 @@
     <col min="2" max="2" width="14.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" style="3" customWidth="1"/>
     <col min="12" max="12" width="21.75" style="3" customWidth="1"/>
-    <col min="13" max="13" width="9" style="10" customWidth="1"/>
+    <col min="13" max="13" width="9" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2266,25 +1654,25 @@
       <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="5">
         <v>4</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="6">
         <v>44399.549432870372</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="17"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2299,25 +1687,25 @@
       <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="5">
         <v>4</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="6">
         <v>44399.555428240739</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="17"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2332,25 +1720,25 @@
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="5">
         <v>17.600000000000001</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="6">
         <v>44495.444791666669</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="17"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2365,25 +1753,25 @@
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="5">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="6">
         <v>44495.562280092592</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="17"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2398,25 +1786,25 @@
       <c r="D6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="5">
         <v>57.7</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="6">
         <v>44517.329583333332</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="17"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2431,25 +1819,25 @@
       <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="5">
         <v>1000000</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="6">
         <v>44525.528923611113</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="17"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -2464,25 +1852,25 @@
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="5">
         <v>30.3</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="6">
         <v>44544.481157407405</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="17"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2497,25 +1885,25 @@
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="5">
         <v>19.5</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="6">
         <v>44566.391747685186</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="17"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -2530,25 +1918,25 @@
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="5">
         <v>18.3</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="6">
         <v>44566.391805555555</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="17"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2563,25 +1951,25 @@
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="5">
         <v>23.56</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="6">
         <v>44625.391805555555</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="17"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2602,7 +1990,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D44829-4A1B-44BC-99D3-A38FF6D79AF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2612,54 +2000,54 @@
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.75" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2">
         <f>COUNTIFS(Tickets!J1:J990, "00")</f>
         <v>0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2">
         <f>COUNTIFS(Tickets!J1:J990, "01")</f>
         <v>0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2">
         <f>COUNTIFS(Tickets!J1:J990, "02")</f>
         <v>0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2">
         <f>COUNTIFS(Tickets!J1:J990, "03")</f>
         <v>0</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
         <f>COUNTIFS(Tickets!J1:K990, "98")</f>
         <v>0</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2">
         <f>COUNTIFS(Tickets!J1:L990, "99")</f>
         <v>0</v>
       </c>

</xml_diff>